<commit_message>
modified:   Extractor.py modified:   Extractor/companies.txt modified:   Extractor/companies.xlsx modified:   Extractor/details.xlsx
</commit_message>
<xml_diff>
--- a/Extractor/companies.xlsx
+++ b/Extractor/companies.xlsx
@@ -1306,7 +1306,7 @@
   <dimension ref="A1:L203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.142857142857141" defaultRowHeight="15"/>
@@ -1965,28 +1965,1228 @@
           <t>Seagoville</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>TX</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>5576 N Interstate Highway 45</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="0" t="inlineStr">
         <is>
           <t>Ennis</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="0" t="inlineStr">
         <is>
           <t>Tx</t>
         </is>
       </c>
       <c r="L16" s="0" t="n">
         <v>115</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>El Tule Properties Llc</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>803 Brandon Drive</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>13 White Rock Trl</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>Allen</t>
+        </is>
+      </c>
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>True North Property Owner</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>808 Dakota Lane</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>PO Box 4090</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>Scottsdale</t>
+        </is>
+      </c>
+      <c r="G18" s="0" t="inlineStr">
+        <is>
+          <t>Az</t>
+        </is>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>Sfr 1 2021 1 Borrower Llc</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>1625 Emily Lane</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>1508 Brookhollow Dr</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>Santa Ana</t>
+        </is>
+      </c>
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>Safari One Asset Company Llc</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>1611 Emily Lane</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>5001 Plaza On The Lk Ste 200</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>Austin</t>
+        </is>
+      </c>
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>Home Sfr Borrower Llc</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>813 Huddleston Court</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>3505 Kroger Blvd</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>Duluth</t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>Ga</t>
+        </is>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>Amc Homes Llc</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>1002 Fawn Meadow Drive</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>415 Estate Ln</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>Terrell</t>
+        </is>
+      </c>
+      <c r="G22" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>Rental Transition Llc</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>1519 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>8765 Cleaver Ln</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>Terrell</t>
+        </is>
+      </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>Smfamilyholdings Llc</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>1516 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>7505 Vista Ridge Ct</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>Garland</t>
+        </is>
+      </c>
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>1514 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G25" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>1512 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G26" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>1510 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G27" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>Md Thompson Leasing Company 4</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>1508 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E28" s="0" t="inlineStr">
+        <is>
+          <t>1918 Seagoville Rd</t>
+        </is>
+      </c>
+      <c r="F28" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="G28" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>1506 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E29" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F29" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G29" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>Md Thompson Leasing Company 4</t>
+        </is>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>1504 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E30" s="0" t="inlineStr">
+        <is>
+          <t>1918 Seagoville Rd</t>
+        </is>
+      </c>
+      <c r="F30" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="G30" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>1502 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E31" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F31" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G31" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>El Tule Properties Llc</t>
+        </is>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>803 Brandon Drive</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E32" s="0" t="inlineStr">
+        <is>
+          <t>13 White Rock Trl</t>
+        </is>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
+        <is>
+          <t>Allen</t>
+        </is>
+      </c>
+      <c r="G32" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>True North Property Owner</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>808 Dakota Lane</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E33" s="0" t="inlineStr">
+        <is>
+          <t>PO Box 4090</t>
+        </is>
+      </c>
+      <c r="F33" s="0" t="inlineStr">
+        <is>
+          <t>Scottsdale</t>
+        </is>
+      </c>
+      <c r="G33" s="0" t="inlineStr">
+        <is>
+          <t>Az</t>
+        </is>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>Sfr 1 2021 1 Borrower Llc</t>
+        </is>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>1625 Emily Lane</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E34" s="0" t="inlineStr">
+        <is>
+          <t>1508 Brookhollow Dr</t>
+        </is>
+      </c>
+      <c r="F34" s="0" t="inlineStr">
+        <is>
+          <t>Santa Ana</t>
+        </is>
+      </c>
+      <c r="G34" s="0" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>Safari One Asset Company Llc</t>
+        </is>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>1611 Emily Lane</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E35" s="0" t="inlineStr">
+        <is>
+          <t>5001 Plaza On The Lk Ste 200</t>
+        </is>
+      </c>
+      <c r="F35" s="0" t="inlineStr">
+        <is>
+          <t>Austin</t>
+        </is>
+      </c>
+      <c r="G35" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>Home Sfr Borrower Llc</t>
+        </is>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>813 Huddleston Court</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E36" s="0" t="inlineStr">
+        <is>
+          <t>3505 Kroger Blvd</t>
+        </is>
+      </c>
+      <c r="F36" s="0" t="inlineStr">
+        <is>
+          <t>Duluth</t>
+        </is>
+      </c>
+      <c r="G36" s="0" t="inlineStr">
+        <is>
+          <t>Ga</t>
+        </is>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>Amc Homes Llc</t>
+        </is>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>1002 Fawn Meadow Drive</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E37" s="0" t="inlineStr">
+        <is>
+          <t>415 Estate Ln</t>
+        </is>
+      </c>
+      <c r="F37" s="0" t="inlineStr">
+        <is>
+          <t>Terrell</t>
+        </is>
+      </c>
+      <c r="G37" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>Rental Transition Llc</t>
+        </is>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>1519 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E38" s="0" t="inlineStr">
+        <is>
+          <t>8765 Cleaver Ln</t>
+        </is>
+      </c>
+      <c r="F38" s="0" t="inlineStr">
+        <is>
+          <t>Terrell</t>
+        </is>
+      </c>
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>Smfamilyholdings Llc</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>1516 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E39" s="0" t="inlineStr">
+        <is>
+          <t>7505 Vista Ridge Ct</t>
+        </is>
+      </c>
+      <c r="F39" s="0" t="inlineStr">
+        <is>
+          <t>Garland</t>
+        </is>
+      </c>
+      <c r="G39" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>1514 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E40" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F40" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G40" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>1512 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E41" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F41" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>1510 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E42" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F42" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G42" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>Md Thompson Leasing Company 4</t>
+        </is>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>1508 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E43" s="0" t="inlineStr">
+        <is>
+          <t>1918 Seagoville Rd</t>
+        </is>
+      </c>
+      <c r="F43" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="G43" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>1506 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G44" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L44" s="0" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>Md Thompson Leasing Company 4</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>1504 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
+        <is>
+          <t>1918 Seagoville Rd</t>
+        </is>
+      </c>
+      <c r="F45" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="G45" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L45" s="0" t="n">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>City &amp;amp; Cntry Hms Of America Llc</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>1502 La Fonda Drive</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>Seagoville</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr">
+        <is>
+          <t>5576 N Interstate Highway 45</t>
+        </is>
+      </c>
+      <c r="F46" s="0" t="inlineStr">
+        <is>
+          <t>Ennis</t>
+        </is>
+      </c>
+      <c r="G46" s="0" t="inlineStr">
+        <is>
+          <t>Tx</t>
+        </is>
+      </c>
+      <c r="L46" s="0" t="n">
+        <v>343</v>
       </c>
     </row>
     <row r="102">

</xml_diff>